<commit_message>
dodanie kolejkowania graczy i wyboru trybów
</commit_message>
<xml_diff>
--- a/noncode/zasady.xlsx
+++ b/noncode/zasady.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shoyun\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mikołaj\Desktop\warcaby\noncode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC58B60-9AAE-45D9-BB22-9061E1A4FA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF1D471-4CE8-4626-B5DD-3CC2CCDD10BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="0" windowWidth="28755" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
   <si>
     <t>warcaby polskie (międzynarodowe)</t>
   </si>
@@ -53,18 +53,9 @@
     <t>pionków</t>
   </si>
   <si>
-    <t>po 10</t>
-  </si>
-  <si>
-    <t>poruszanie</t>
-  </si>
-  <si>
     <t>1 do przodu po przekątnej</t>
   </si>
   <si>
-    <t>bicie</t>
-  </si>
-  <si>
     <t>do przodu i do tyłu</t>
   </si>
   <si>
@@ -86,9 +77,6 @@
     <t>remis</t>
   </si>
   <si>
-    <t>15 ruchów damką bez bicia</t>
-  </si>
-  <si>
     <t>warcaby angielskie (amerykańskie)</t>
   </si>
   <si>
@@ -98,21 +86,12 @@
     <t>po 12</t>
   </si>
   <si>
-    <t>do przodu</t>
-  </si>
-  <si>
     <t>damki (królowie)</t>
   </si>
   <si>
     <t>?</t>
   </si>
   <si>
-    <t>obowiązkowe, do końca</t>
-  </si>
-  <si>
-    <t>warcaby dwuliniowe</t>
-  </si>
-  <si>
     <t>po 8</t>
   </si>
   <si>
@@ -122,9 +101,6 @@
     <t xml:space="preserve">W jednym ruchu wolno wykonać więcej niż jeden skok tym samym pionkiem, przeskakując przez kolejne pionki/królówki (damki) przeciwnika, także do tyłu w kolejnych biciach pionkiem. </t>
   </si>
   <si>
-    <t>do przodu i do tyłu (?)</t>
-  </si>
-  <si>
     <t>opcjonalnie:</t>
   </si>
   <si>
@@ -155,21 +131,6 @@
     <t>Jeśli gracz nie zauważy swojej możliwości bicia, pionek który mógł je wykonać jest usuwany z planszy jeśli przeciwnik zauważy ten fakt na samym początku swojego ruchu (max. 5 sekund)</t>
   </si>
   <si>
-    <t>poruszają się też do tyłu</t>
-  </si>
-  <si>
-    <t>biją też do tyłu</t>
-  </si>
-  <si>
-    <t>nie potrzebuje przeskoczyć (?)</t>
-  </si>
-  <si>
-    <t>muszą przeskoczyć do bicia</t>
-  </si>
-  <si>
-    <t>obowiązkowe, maksymalne</t>
-  </si>
-  <si>
     <t>Notacja (zapis partii i pozycji): Partie i pozycje w warcabach polskich zapisuje się korzystając ze specjalnej notacji (sposobu zapisu) wynalezionej w XVIII w. przez Francuza C. Manoury. Dla celów notacji czarne pola planszy (warcabnicy) do gry w warcaby polskie numeruje się począwszy od skrajnego prawego pola od strony grającego czarnymi kamieniami liczbami od 1 do 50. Prawe skrajne pole, patrząc od strony grającego białymi, ma wówczas numer 50. Posunięcia zapisuje się podając numer pola początkowego i pola końcowego rozdzielone znakiem „-” np. 01-06. Przy zapisie pozycji podajemy numery pól, na których znajdują się kamienie, np.</t>
   </si>
   <si>
@@ -180,13 +141,43 @@
   </si>
   <si>
     <t>Przy czym zwykłe kamienie oznaczone są tylko numerem pola, na którym się znajdują, zaś damki wykazujemy pisząc numer pola i dodając (D).</t>
+  </si>
+  <si>
+    <t>po 20</t>
+  </si>
+  <si>
+    <t>poruszanie pionków</t>
+  </si>
+  <si>
+    <t>bicie pionkami</t>
+  </si>
+  <si>
+    <t>obowiązkowe</t>
+  </si>
+  <si>
+    <t>TYLKO do przodu</t>
+  </si>
+  <si>
+    <t>biją we wszystkich kierunkach</t>
+  </si>
+  <si>
+    <t>poruszają się o JEDNO pole we wszystkich kierunkach</t>
+  </si>
+  <si>
+    <t>warcaby tajskie</t>
+  </si>
+  <si>
+    <t>po zbiciu zatrzymuje się za pionkiem</t>
+  </si>
+  <si>
+    <t>https://www.draughtsforandroid.com/pl/nowosci/warcaby-rozne-zasady-gry-54.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,6 +206,15 @@
       <name val="Georgia"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -338,10 +338,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -388,31 +389,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -428,9 +433,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -468,7 +473,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -574,7 +579,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -727,18 +732,20 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="1" customWidth="1"/>
-    <col min="2" max="4" width="40.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" style="19" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" style="16" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -746,13 +753,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -760,221 +767,224 @@
         <v>3</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="C4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="22"/>
+      <c r="B6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="23"/>
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="22"/>
+      <c r="B9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="3" t="s">
+      <c r="C9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="22"/>
+      <c r="B10" s="12" t="s">
         <v>43</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="12" t="s">
-        <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D13" s="24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="1.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="1:5" ht="238.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="20"/>
+      <c r="D23" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
+      <c r="B24" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="D24" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="20"/>
+      <c r="B25" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D13" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D14" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E16" s="21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="1.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E22" s="15"/>
-    </row>
-    <row r="23" spans="1:5" ht="238.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="23"/>
-      <c r="B24" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="23"/>
-      <c r="B25" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="23"/>
-      <c r="D25" s="14" t="s">
+    <row r="26" spans="1:5" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
+      <c r="B26" s="19" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="23"/>
-      <c r="B26" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="23"/>
+      <c r="C26" s="20"/>
       <c r="D26" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
       <c r="D27" s="14" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -982,7 +992,10 @@
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A8:A10"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D13" r:id="rId1" xr:uid="{07AF6C3B-540C-43C4-A515-0979EC202E49}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>